<commit_message>
Created CSV files and updated Excel file w/ new columns
</commit_message>
<xml_diff>
--- a/RepData/DataSources v2.xlsx
+++ b/RepData/DataSources v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\iCloudDrive\Data Bootcamp\Module 06 - Final Project\Group-5\RepData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76589162-9AFB-4715-AAFF-B3EB1FA6C474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555AB787-62C6-4B67-A8F3-43FA2716CCC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25515" yWindow="510" windowWidth="24210" windowHeight="14550" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="1245" windowWidth="22800" windowHeight="14055" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="3" r:id="rId1"/>
@@ -18111,7 +18111,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
@@ -18125,8 +18125,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -18486,7 +18484,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18670,9 +18668,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA1135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomLeft" activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32970,7 +32968,7 @@
       <c r="A327" t="s">
         <v>275</v>
       </c>
-      <c r="B327" s="9" t="s">
+      <c r="B327" t="s">
         <v>276</v>
       </c>
       <c r="C327" t="s">
@@ -33030,7 +33028,7 @@
       <c r="A328" t="s">
         <v>2052</v>
       </c>
-      <c r="B328" s="9" t="s">
+      <c r="B328" t="s">
         <v>2053</v>
       </c>
       <c r="C328" t="s">
@@ -33077,7 +33075,7 @@
       <c r="A329" t="s">
         <v>577</v>
       </c>
-      <c r="B329" s="9" t="s">
+      <c r="B329" t="s">
         <v>578</v>
       </c>
       <c r="C329" t="s">
@@ -33134,7 +33132,7 @@
       <c r="A330" t="s">
         <v>1989</v>
       </c>
-      <c r="B330" s="9" t="s">
+      <c r="B330" t="s">
         <v>1990</v>
       </c>
       <c r="C330" t="s">
@@ -33181,7 +33179,7 @@
       <c r="A331" t="s">
         <v>1812</v>
       </c>
-      <c r="B331" s="9" t="s">
+      <c r="B331" t="s">
         <v>1813</v>
       </c>
       <c r="C331" t="s">
@@ -33228,7 +33226,7 @@
       <c r="A332" t="s">
         <v>1368</v>
       </c>
-      <c r="B332" s="9" t="s">
+      <c r="B332" t="s">
         <v>1369</v>
       </c>
       <c r="C332" t="s">
@@ -33281,7 +33279,7 @@
       <c r="A333" t="s">
         <v>141</v>
       </c>
-      <c r="B333" s="9" t="s">
+      <c r="B333" t="s">
         <v>142</v>
       </c>
       <c r="C333" t="s">
@@ -33328,7 +33326,7 @@
       <c r="A334" t="s">
         <v>1636</v>
       </c>
-      <c r="B334" s="9" t="s">
+      <c r="B334" t="s">
         <v>1637</v>
       </c>
       <c r="C334" t="s">
@@ -33385,7 +33383,7 @@
       <c r="A335" t="s">
         <v>2173</v>
       </c>
-      <c r="B335" s="9" t="s">
+      <c r="B335" t="s">
         <v>2174</v>
       </c>
       <c r="C335" t="s">
@@ -33432,7 +33430,7 @@
       <c r="A336" t="s">
         <v>1952</v>
       </c>
-      <c r="B336" s="9" t="s">
+      <c r="B336" t="s">
         <v>1953</v>
       </c>
       <c r="C336" t="s">
@@ -33479,7 +33477,7 @@
       <c r="A337" t="s">
         <v>4186</v>
       </c>
-      <c r="B337" s="9" t="s">
+      <c r="B337" t="s">
         <v>4187</v>
       </c>
       <c r="C337" t="s">
@@ -33526,7 +33524,7 @@
       <c r="A338" t="s">
         <v>1698</v>
       </c>
-      <c r="B338" s="9" t="s">
+      <c r="B338" t="s">
         <v>1699</v>
       </c>
       <c r="C338" t="s">
@@ -33573,7 +33571,7 @@
       <c r="A339" t="s">
         <v>2098</v>
       </c>
-      <c r="B339" s="9" t="s">
+      <c r="B339" t="s">
         <v>2099</v>
       </c>
       <c r="C339" t="s">
@@ -33620,7 +33618,7 @@
       <c r="A340" t="s">
         <v>864</v>
       </c>
-      <c r="B340" s="9" t="s">
+      <c r="B340" t="s">
         <v>865</v>
       </c>
       <c r="C340" t="s">
@@ -33677,7 +33675,7 @@
       <c r="A341" t="s">
         <v>1856</v>
       </c>
-      <c r="B341" s="9" t="s">
+      <c r="B341" t="s">
         <v>1857</v>
       </c>
       <c r="C341" t="s">
@@ -33724,7 +33722,7 @@
       <c r="A342" t="s">
         <v>1041</v>
       </c>
-      <c r="B342" s="9" t="s">
+      <c r="B342" t="s">
         <v>1042</v>
       </c>
       <c r="C342" t="s">
@@ -33774,7 +33772,7 @@
       <c r="A343" t="s">
         <v>4205</v>
       </c>
-      <c r="B343" s="9" t="s">
+      <c r="B343" t="s">
         <v>4206</v>
       </c>
       <c r="C343" t="s">
@@ -33821,7 +33819,7 @@
       <c r="A344" t="s">
         <v>902</v>
       </c>
-      <c r="B344" s="9" t="s">
+      <c r="B344" t="s">
         <v>903</v>
       </c>
       <c r="C344" t="s">
@@ -33868,7 +33866,7 @@
       <c r="A345" t="s">
         <v>959</v>
       </c>
-      <c r="B345" s="9" t="s">
+      <c r="B345" t="s">
         <v>960</v>
       </c>
       <c r="C345" t="s">
@@ -33915,7 +33913,7 @@
       <c r="A346" t="s">
         <v>1005</v>
       </c>
-      <c r="B346" s="9" t="s">
+      <c r="B346" t="s">
         <v>1006</v>
       </c>
       <c r="C346" t="s">
@@ -33965,7 +33963,7 @@
       <c r="A347" t="s">
         <v>2196</v>
       </c>
-      <c r="B347" s="9" t="s">
+      <c r="B347" t="s">
         <v>2197</v>
       </c>
       <c r="C347" t="s">
@@ -34025,7 +34023,7 @@
       <c r="A348" t="s">
         <v>1124</v>
       </c>
-      <c r="B348" s="9" t="s">
+      <c r="B348" t="s">
         <v>1125</v>
       </c>
       <c r="C348" t="s">
@@ -34072,7 +34070,7 @@
       <c r="A349" t="s">
         <v>1520</v>
       </c>
-      <c r="B349" s="9" t="s">
+      <c r="B349" t="s">
         <v>1521</v>
       </c>
       <c r="C349" t="s">
@@ -34119,7 +34117,7 @@
       <c r="A350" t="s">
         <v>740</v>
       </c>
-      <c r="B350" s="9" t="s">
+      <c r="B350" t="s">
         <v>741</v>
       </c>
       <c r="C350" t="s">
@@ -34166,7 +34164,7 @@
       <c r="A351" t="s">
         <v>2505</v>
       </c>
-      <c r="B351" s="9" t="s">
+      <c r="B351" t="s">
         <v>2506</v>
       </c>
       <c r="C351" t="s">
@@ -34213,7 +34211,7 @@
       <c r="A352" t="s">
         <v>1580</v>
       </c>
-      <c r="B352" s="9" t="s">
+      <c r="B352" t="s">
         <v>1581</v>
       </c>
       <c r="C352" t="s">
@@ -34263,7 +34261,7 @@
       <c r="A353" t="s">
         <v>562</v>
       </c>
-      <c r="B353" s="9" t="s">
+      <c r="B353" t="s">
         <v>563</v>
       </c>
       <c r="C353" t="s">
@@ -34310,7 +34308,7 @@
       <c r="A354" t="s">
         <v>1630</v>
       </c>
-      <c r="B354" s="9" t="s">
+      <c r="B354" t="s">
         <v>1631</v>
       </c>
       <c r="C354" t="s">
@@ -34357,7 +34355,7 @@
       <c r="A355" t="s">
         <v>2307</v>
       </c>
-      <c r="B355" s="10" t="s">
+      <c r="B355" s="2" t="s">
         <v>2308</v>
       </c>
       <c r="C355" t="s">
@@ -34404,7 +34402,7 @@
       <c r="A356" t="s">
         <v>699</v>
       </c>
-      <c r="B356" s="9" t="s">
+      <c r="B356" t="s">
         <v>700</v>
       </c>
       <c r="C356" t="s">
@@ -34451,7 +34449,7 @@
       <c r="A357" t="s">
         <v>1683</v>
       </c>
-      <c r="B357" s="9" t="s">
+      <c r="B357" t="s">
         <v>1684</v>
       </c>
       <c r="C357" t="s">
@@ -34498,7 +34496,7 @@
       <c r="A358" t="s">
         <v>4228</v>
       </c>
-      <c r="B358" s="9" t="s">
+      <c r="B358" t="s">
         <v>4229</v>
       </c>
       <c r="C358" t="s">
@@ -34545,7 +34543,7 @@
       <c r="A359" t="s">
         <v>1427</v>
       </c>
-      <c r="B359" s="9" t="s">
+      <c r="B359" t="s">
         <v>1428</v>
       </c>
       <c r="C359" t="s">
@@ -34592,7 +34590,7 @@
       <c r="A360" t="s">
         <v>2250</v>
       </c>
-      <c r="B360" s="9" t="s">
+      <c r="B360" t="s">
         <v>2251</v>
       </c>
       <c r="C360" t="s">
@@ -34639,7 +34637,7 @@
       <c r="A361" t="s">
         <v>753</v>
       </c>
-      <c r="B361" s="9" t="s">
+      <c r="B361" t="s">
         <v>754</v>
       </c>
       <c r="C361" t="s">
@@ -34686,7 +34684,7 @@
       <c r="A362" t="s">
         <v>2241</v>
       </c>
-      <c r="B362" s="9" t="s">
+      <c r="B362" t="s">
         <v>2242</v>
       </c>
       <c r="C362" t="s">
@@ -34733,7 +34731,7 @@
       <c r="A363" t="s">
         <v>802</v>
       </c>
-      <c r="B363" s="9" t="s">
+      <c r="B363" t="s">
         <v>803</v>
       </c>
       <c r="C363" t="s">
@@ -34783,7 +34781,7 @@
       <c r="A364" t="s">
         <v>1179</v>
       </c>
-      <c r="B364" s="9" t="s">
+      <c r="B364" t="s">
         <v>1180</v>
       </c>
       <c r="C364" t="s">
@@ -34830,7 +34828,7 @@
       <c r="A365" t="s">
         <v>424</v>
       </c>
-      <c r="B365" s="9" t="s">
+      <c r="B365" t="s">
         <v>425</v>
       </c>
       <c r="C365" t="s">
@@ -34877,7 +34875,7 @@
       <c r="A366" t="s">
         <v>1956</v>
       </c>
-      <c r="B366" s="9" t="s">
+      <c r="B366" t="s">
         <v>1957</v>
       </c>
       <c r="C366" t="s">
@@ -34924,7 +34922,7 @@
       <c r="A367" t="s">
         <v>830</v>
       </c>
-      <c r="B367" s="9" t="s">
+      <c r="B367" t="s">
         <v>831</v>
       </c>
       <c r="C367" t="s">
@@ -34971,7 +34969,7 @@
       <c r="A368" t="s">
         <v>582</v>
       </c>
-      <c r="B368" s="9" t="s">
+      <c r="B368" t="s">
         <v>583</v>
       </c>
       <c r="C368" t="s">
@@ -35018,7 +35016,7 @@
       <c r="A369" t="s">
         <v>2385</v>
       </c>
-      <c r="B369" s="9" t="s">
+      <c r="B369" t="s">
         <v>2386</v>
       </c>
       <c r="C369" t="s">
@@ -35071,7 +35069,7 @@
       <c r="A370" t="s">
         <v>4255</v>
       </c>
-      <c r="B370" s="9" t="s">
+      <c r="B370" t="s">
         <v>4256</v>
       </c>
       <c r="C370" t="s">
@@ -35118,7 +35116,7 @@
       <c r="A371" t="s">
         <v>1803</v>
       </c>
-      <c r="B371" s="9" t="s">
+      <c r="B371" t="s">
         <v>1804</v>
       </c>
       <c r="C371" t="s">
@@ -35165,7 +35163,7 @@
       <c r="A372" t="s">
         <v>556</v>
       </c>
-      <c r="B372" s="9" t="s">
+      <c r="B372" t="s">
         <v>557</v>
       </c>
       <c r="C372" t="s">
@@ -35212,7 +35210,7 @@
       <c r="A373" t="s">
         <v>922</v>
       </c>
-      <c r="B373" s="9" t="s">
+      <c r="B373" t="s">
         <v>923</v>
       </c>
       <c r="C373" t="s">
@@ -35259,7 +35257,7 @@
       <c r="A374" t="s">
         <v>411</v>
       </c>
-      <c r="B374" s="9" t="s">
+      <c r="B374" t="s">
         <v>412</v>
       </c>
       <c r="C374" t="s">
@@ -35306,7 +35304,7 @@
       <c r="A375" t="s">
         <v>419</v>
       </c>
-      <c r="B375" s="9" t="s">
+      <c r="B375" t="s">
         <v>420</v>
       </c>
       <c r="C375" t="s">
@@ -35356,7 +35354,7 @@
       <c r="A376" t="s">
         <v>1622</v>
       </c>
-      <c r="B376" s="9" t="s">
+      <c r="B376" t="s">
         <v>1623</v>
       </c>
       <c r="C376" t="s">
@@ -35403,7 +35401,7 @@
       <c r="A377" t="s">
         <v>1377</v>
       </c>
-      <c r="B377" s="9" t="s">
+      <c r="B377" t="s">
         <v>1378</v>
       </c>
       <c r="C377" t="s">
@@ -35450,7 +35448,7 @@
       <c r="A378" t="s">
         <v>1148</v>
       </c>
-      <c r="B378" s="9" t="s">
+      <c r="B378" t="s">
         <v>1149</v>
       </c>
       <c r="C378" t="s">
@@ -35497,7 +35495,7 @@
       <c r="A379" t="s">
         <v>748</v>
       </c>
-      <c r="B379" s="9" t="s">
+      <c r="B379" t="s">
         <v>749</v>
       </c>
       <c r="C379" t="s">
@@ -35544,7 +35542,7 @@
       <c r="A380" t="s">
         <v>206</v>
       </c>
-      <c r="B380" s="9" t="s">
+      <c r="B380" t="s">
         <v>207</v>
       </c>
       <c r="C380" t="s">
@@ -35591,7 +35589,7 @@
       <c r="A381" t="s">
         <v>636</v>
       </c>
-      <c r="B381" s="10" t="s">
+      <c r="B381" s="2" t="s">
         <v>637</v>
       </c>
       <c r="C381" t="s">
@@ -35641,7 +35639,7 @@
       <c r="A382" t="s">
         <v>2126</v>
       </c>
-      <c r="B382" s="9" t="s">
+      <c r="B382" t="s">
         <v>2127</v>
       </c>
       <c r="C382" t="s">
@@ -35691,7 +35689,7 @@
       <c r="A383" t="s">
         <v>1681</v>
       </c>
-      <c r="B383" s="9" t="s">
+      <c r="B383" t="s">
         <v>1682</v>
       </c>
       <c r="C383" t="s">
@@ -35738,7 +35736,7 @@
       <c r="A384" t="s">
         <v>1768</v>
       </c>
-      <c r="B384" s="9" t="s">
+      <c r="B384" t="s">
         <v>1769</v>
       </c>
       <c r="C384" t="s">
@@ -35785,7 +35783,7 @@
       <c r="A385" t="s">
         <v>2222</v>
       </c>
-      <c r="B385" s="9" t="s">
+      <c r="B385" t="s">
         <v>2223</v>
       </c>
       <c r="C385" t="s">
@@ -35832,7 +35830,7 @@
       <c r="A386" t="s">
         <v>2448</v>
       </c>
-      <c r="B386" s="9" t="s">
+      <c r="B386" t="s">
         <v>2449</v>
       </c>
       <c r="C386" t="s">
@@ -35879,7 +35877,7 @@
       <c r="A387" t="s">
         <v>2443</v>
       </c>
-      <c r="B387" s="9" t="s">
+      <c r="B387" t="s">
         <v>2444</v>
       </c>
       <c r="C387" t="s">
@@ -35926,7 +35924,7 @@
       <c r="A388" t="s">
         <v>184</v>
       </c>
-      <c r="B388" s="9" t="s">
+      <c r="B388" t="s">
         <v>185</v>
       </c>
       <c r="C388" t="s">
@@ -35973,7 +35971,7 @@
       <c r="A389" t="s">
         <v>1773</v>
       </c>
-      <c r="B389" s="9" t="s">
+      <c r="B389" t="s">
         <v>1774</v>
       </c>
       <c r="C389" t="s">
@@ -36020,7 +36018,7 @@
       <c r="A390" t="s">
         <v>2357</v>
       </c>
-      <c r="B390" s="9" t="s">
+      <c r="B390" t="s">
         <v>2358</v>
       </c>
       <c r="C390" t="s">
@@ -44492,7 +44490,7 @@
       <c r="V568" t="s">
         <v>4904</v>
       </c>
-      <c r="W568" s="9" t="s">
+      <c r="W568" t="s">
         <v>3807</v>
       </c>
       <c r="X568" t="str">
@@ -69372,7 +69370,7 @@
         <v>01</v>
       </c>
       <c r="R1090" t="str">
-        <f t="shared" ref="R1090:R1153" si="71">_xlfn.CONCAT(P1090,Q1090)</f>
+        <f t="shared" ref="R1090:R1135" si="71">_xlfn.CONCAT(P1090,Q1090)</f>
         <v>WA01</v>
       </c>
       <c r="S1090" t="s">

</xml_diff>